<commit_message>
Fixed Water tolerance columns
</commit_message>
<xml_diff>
--- a/Data/VegData.xlsx
+++ b/Data/VegData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="920" windowWidth="25460" windowHeight="13260" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="920" windowWidth="25460" windowHeight="13260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -732,12 +732,6 @@
     <t>Water tolerance max</t>
   </si>
   <si>
-    <t>Wtmin (cm)</t>
-  </si>
-  <si>
-    <t>Wtmax(cm)</t>
-  </si>
-  <si>
     <t>The number of wet months</t>
   </si>
   <si>
@@ -805,6 +799,12 @@
   </si>
   <si>
     <t>https://www.fs.fed.us/database/feis/plants/shrub/pruili/all.html</t>
+  </si>
+  <si>
+    <t>WTmin (cm)</t>
+  </si>
+  <si>
+    <t>WTmax(cm)</t>
   </si>
 </sst>
 </file>
@@ -967,6 +967,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -988,7 +989,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1275,7 +1275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1578,7 +1578,7 @@
         <v>47</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G6" s="5">
         <v>13</v>
@@ -1608,7 +1608,7 @@
         <v>183</v>
       </c>
       <c r="P6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -1658,7 +1658,7 @@
         <v>225</v>
       </c>
       <c r="P7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="Q7" t="s">
         <v>124</v>
@@ -1711,7 +1711,7 @@
         <v>184</v>
       </c>
       <c r="P8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="Q8" t="s">
         <v>125</v>
@@ -1734,7 +1734,7 @@
         <v>48</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G9" s="5">
         <v>28</v>
@@ -1764,7 +1764,7 @@
         <v>185</v>
       </c>
       <c r="P9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Q9" t="s">
         <v>111</v>
@@ -1840,7 +1840,7 @@
         <v>48</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G11" s="5">
         <v>28</v>
@@ -1870,7 +1870,7 @@
         <v>223</v>
       </c>
       <c r="P11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="Q11" t="s">
         <v>126</v>
@@ -2011,7 +2011,7 @@
         <v>192</v>
       </c>
       <c r="P14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Q14" t="s">
         <v>129</v>
@@ -2108,7 +2108,7 @@
         <v>195</v>
       </c>
       <c r="P16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="Q16" t="s">
         <v>118</v>
@@ -2161,7 +2161,7 @@
         <v>196</v>
       </c>
       <c r="P17" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="Q17" t="s">
         <v>111</v>
@@ -2214,7 +2214,7 @@
         <v>198</v>
       </c>
       <c r="P18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Q18" t="s">
         <v>130</v>
@@ -2458,7 +2458,7 @@
         <v>205</v>
       </c>
       <c r="P23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Q23" t="s">
         <v>136</v>
@@ -2481,7 +2481,7 @@
         <v>47</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G24" s="5">
         <v>28</v>
@@ -2511,7 +2511,7 @@
         <v>208</v>
       </c>
       <c r="P24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="Q24" t="s">
         <v>137</v>
@@ -2534,7 +2534,7 @@
         <v>48</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G25" s="5">
         <v>28</v>
@@ -2564,7 +2564,7 @@
         <v>209</v>
       </c>
       <c r="P25" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="Q25" t="s">
         <v>119</v>
@@ -3091,8 +3091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3104,10 +3104,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="22"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
@@ -3163,13 +3163,13 @@
     </row>
     <row r="7" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>231</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="8" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
-        <v>234</v>
+        <v>257</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>232</v>
@@ -3193,8 +3193,8 @@
       <c r="B9" t="s">
         <v>189</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>235</v>
+      <c r="C9" s="22" t="s">
+        <v>233</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -3256,10 +3256,10 @@
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="24"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -3310,44 +3310,44 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>237</v>
-      </c>
-      <c r="D22" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="D22" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>238</v>
-      </c>
-      <c r="D23" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="D23" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
@@ -3356,36 +3356,36 @@
         <v>156</v>
       </c>
       <c r="C24" t="s">
-        <v>239</v>
-      </c>
-      <c r="D24" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="D24" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>240</v>
-      </c>
-      <c r="D25" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="D25" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="27"/>
+      <c r="C27" s="28"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
@@ -3444,10 +3444,10 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="C36" s="24"/>
+      <c r="C36" s="25"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -3457,36 +3457,36 @@
       <c r="B37" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Forgot to delete something
</commit_message>
<xml_diff>
--- a/Data/VegData.xlsx
+++ b/Data/VegData.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="440" yWindow="580" windowWidth="26880" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="580" windowWidth="26880" windowHeight="13600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="Data_Description" sheetId="2" r:id="rId3"/>
+    <sheet name="Data_Description" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$A$41</definedName>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="372">
   <si>
     <t>SN</t>
   </si>
@@ -1204,9 +1203,6 @@
       </rPr>
       <t>.  Plants that prefer soils that are moist year round. (These are riparian plants tend to grow in or near creeks, seeps, or near rivers or lakes.) Once established, these plants should still thrive with little or no additional irrigation in years of normal precipitation, as long as they are planted in areas with naturally year-round moist soils. If you plant them in drier soils, they’ll need additional irrigation in order to thrive.</t>
     </r>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1426,15 +1422,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1450,9 +1437,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1473,23 +1457,35 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1774,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -1790,7 +1786,7 @@
     <col min="16" max="16" width="11.33203125" style="4" customWidth="1"/>
     <col min="17" max="17" width="10.5" style="4" customWidth="1"/>
     <col min="18" max="18" width="9.6640625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="31.33203125" style="31" customWidth="1"/>
+    <col min="19" max="19" width="31.33203125" style="28" customWidth="1"/>
     <col min="20" max="20" width="39" style="25" customWidth="1"/>
     <col min="21" max="21" width="23.5" style="22" customWidth="1"/>
     <col min="22" max="22" width="24.1640625" style="2" customWidth="1"/>
@@ -1855,10 +1851,10 @@
       <c r="R1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="29" t="s">
+      <c r="S1" s="26" t="s">
         <v>358</v>
       </c>
-      <c r="T1" s="30" t="s">
+      <c r="T1" s="27" t="s">
         <v>257</v>
       </c>
       <c r="U1" s="17" t="s">
@@ -1870,10 +1866,10 @@
       <c r="W1" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="X1" s="37" t="s">
+      <c r="X1" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="Y1" s="32" t="s">
         <v>114</v>
       </c>
       <c r="Z1" s="7"/>
@@ -2560,7 +2556,7 @@
       <c r="R11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="T11" s="32" t="s">
+      <c r="T11" s="29" t="s">
         <v>287</v>
       </c>
       <c r="U11" s="24" t="s">
@@ -2628,7 +2624,7 @@
       <c r="R12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="S12" s="31" t="s">
+      <c r="S12" s="28" t="s">
         <v>309</v>
       </c>
       <c r="U12" s="22" t="s">
@@ -2696,7 +2692,7 @@
       <c r="R13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="T13" s="32"/>
+      <c r="T13" s="29"/>
       <c r="U13" s="22" t="s">
         <v>292</v>
       </c>
@@ -2824,7 +2820,7 @@
       <c r="R15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="S15" s="33" t="s">
+      <c r="S15" s="30" t="s">
         <v>293</v>
       </c>
       <c r="T15" s="25" t="s">
@@ -2895,10 +2891,10 @@
       <c r="R16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="S16" s="33" t="s">
+      <c r="S16" s="30" t="s">
         <v>296</v>
       </c>
-      <c r="T16" s="33" t="s">
+      <c r="T16" s="30" t="s">
         <v>297</v>
       </c>
       <c r="U16" s="22" t="s">
@@ -2969,7 +2965,7 @@
       <c r="R17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="S17" s="33" t="s">
+      <c r="S17" s="30" t="s">
         <v>300</v>
       </c>
       <c r="T17" s="25" t="s">
@@ -3099,7 +3095,7 @@
       <c r="R19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="S19" s="33" t="s">
+      <c r="S19" s="30" t="s">
         <v>302</v>
       </c>
       <c r="U19" s="22" t="s">
@@ -3164,10 +3160,10 @@
       <c r="R20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="S20" s="33" t="s">
+      <c r="S20" s="30" t="s">
         <v>304</v>
       </c>
-      <c r="T20" s="33" t="s">
+      <c r="T20" s="30" t="s">
         <v>305</v>
       </c>
       <c r="U20" s="22" t="s">
@@ -3235,7 +3231,7 @@
       <c r="R21" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="S21" s="31" t="s">
+      <c r="S21" s="28" t="s">
         <v>296</v>
       </c>
       <c r="T21" s="25" t="s">
@@ -3306,7 +3302,7 @@
       <c r="V22" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="X22" s="38" t="s">
+      <c r="X22" s="34" t="s">
         <v>134</v>
       </c>
       <c r="Y22" s="23" t="s">
@@ -3368,7 +3364,7 @@
       <c r="R23" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="S23" s="33" t="s">
+      <c r="S23" s="30" t="s">
         <v>313</v>
       </c>
       <c r="T23" s="25" t="s">
@@ -3442,7 +3438,7 @@
       <c r="R24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="S24" s="33" t="s">
+      <c r="S24" s="30" t="s">
         <v>316</v>
       </c>
       <c r="T24" s="25" t="s">
@@ -3516,10 +3512,10 @@
       <c r="R25" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="S25" s="31" t="s">
+      <c r="S25" s="28" t="s">
         <v>296</v>
       </c>
-      <c r="T25" s="33" t="s">
+      <c r="T25" s="30" t="s">
         <v>319</v>
       </c>
       <c r="U25" s="22" t="s">
@@ -3581,10 +3577,10 @@
       <c r="R26" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="S26" s="33" t="s">
+      <c r="S26" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="T26" s="33" t="s">
+      <c r="T26" s="30" t="s">
         <v>322</v>
       </c>
       <c r="U26" s="24" t="s">
@@ -3649,10 +3645,10 @@
       <c r="R27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="S27" s="33" t="s">
+      <c r="S27" s="30" t="s">
         <v>324</v>
       </c>
-      <c r="T27" s="33" t="s">
+      <c r="T27" s="30" t="s">
         <v>325</v>
       </c>
       <c r="U27" s="24" t="s">
@@ -3720,7 +3716,7 @@
       <c r="R28" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="S28" s="33" t="s">
+      <c r="S28" s="30" t="s">
         <v>328</v>
       </c>
       <c r="T28" s="25" t="s">
@@ -3788,7 +3784,7 @@
       <c r="R29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="S29" s="33" t="s">
+      <c r="S29" s="30" t="s">
         <v>332</v>
       </c>
       <c r="T29" s="25" t="s">
@@ -3859,7 +3855,7 @@
       <c r="R30" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="S30" s="31" t="s">
+      <c r="S30" s="28" t="s">
         <v>335</v>
       </c>
       <c r="T30" s="25" t="s">
@@ -3930,10 +3926,10 @@
       <c r="R31" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="S31" s="31" t="s">
+      <c r="S31" s="28" t="s">
         <v>338</v>
       </c>
-      <c r="T31" s="33" t="s">
+      <c r="T31" s="30" t="s">
         <v>339</v>
       </c>
       <c r="U31" s="24" t="s">
@@ -4001,10 +3997,10 @@
       <c r="R32" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="S32" s="31" t="s">
+      <c r="S32" s="28" t="s">
         <v>341</v>
       </c>
-      <c r="T32" s="33" t="s">
+      <c r="T32" s="30" t="s">
         <v>342</v>
       </c>
       <c r="U32" s="22" t="s">
@@ -4063,7 +4059,7 @@
       <c r="R33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="T33" s="33" t="s">
+      <c r="T33" s="30" t="s">
         <v>345</v>
       </c>
       <c r="U33" s="24" t="s">
@@ -4131,7 +4127,7 @@
       <c r="R34" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="S34" s="31" t="s">
+      <c r="S34" s="28" t="s">
         <v>344</v>
       </c>
       <c r="V34" s="2" t="s">
@@ -4313,432 +4309,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E2:G35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E2" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F2" s="4">
-        <v>2.99</v>
-      </c>
-      <c r="G2">
-        <f>F2*2.54</f>
-        <v>7.5946000000000007</v>
-      </c>
-    </row>
-    <row r="3" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E3" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="F3" s="4">
-        <v>3.49</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G35" si="0">F3*2.54</f>
-        <v>8.8646000000000011</v>
-      </c>
-    </row>
-    <row r="4" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E4" s="4">
-        <v>0.13</v>
-      </c>
-      <c r="F4" s="4">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>10.414</v>
-      </c>
-    </row>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E5" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F5" s="4">
-        <v>3.72</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>9.4488000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E6" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F6" s="4">
-        <v>2.39</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>6.0706000000000007</v>
-      </c>
-    </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E7" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G8" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E9" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F9" s="4">
-        <v>5.94</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>15.087600000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E10" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="F10" s="4">
-        <v>2.96</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>7.5183999999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E11" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F11" s="4">
-        <v>3.08</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>7.8231999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E12" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="F12" s="4">
-        <v>2.23</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>5.6642000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E13" s="4">
-        <v>0.19</v>
-      </c>
-      <c r="F13" s="4">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0.73659999999999992</v>
-      </c>
-    </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E14" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G14" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E15" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F15" s="4">
-        <v>4.46</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>11.3284</v>
-      </c>
-    </row>
-    <row r="16" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E16" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F16" s="4">
-        <v>2.72</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>6.9088000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E17" s="4">
-        <v>0.13</v>
-      </c>
-      <c r="F17" s="4">
-        <v>3.72</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
-        <v>9.4488000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E18" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="G18" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E19" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F19" s="4">
-        <v>2.96</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>7.5183999999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E20" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F20" s="4">
-        <v>52</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
-        <v>132.08000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E21" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F21" s="4">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
-        <v>5.2577999999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E22" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F22" s="4">
-        <v>3</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="0"/>
-        <v>7.62</v>
-      </c>
-    </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E23" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F23" s="4">
-        <v>2.83</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
-        <v>7.1882000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E24" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="F24" s="4">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
-        <v>5.6896000000000004</v>
-      </c>
-    </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E25" s="4">
-        <v>0.13</v>
-      </c>
-      <c r="F25" s="4">
-        <v>3.04</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
-        <v>7.7216000000000005</v>
-      </c>
-    </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E26" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="F26" s="4">
-        <v>2.14</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
-        <v>5.4356</v>
-      </c>
-    </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E27" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F27" s="4">
-        <v>3.04</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
-        <v>7.7216000000000005</v>
-      </c>
-    </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E28" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F28" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
-        <v>5.588000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E29" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="F29" s="4">
-        <v>3.31</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
-        <v>8.4074000000000009</v>
-      </c>
-    </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E30" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F30" s="4">
-        <v>3.61</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="0"/>
-        <v>9.1693999999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E31" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F31" s="4">
-        <v>3.87</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="0"/>
-        <v>9.8298000000000005</v>
-      </c>
-    </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E32" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F32" s="4">
-        <v>2.64</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="0"/>
-        <v>6.7056000000000004</v>
-      </c>
-    </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E33" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="G33" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E34" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="F34" s="4">
-        <v>2.78</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="0"/>
-        <v>7.0611999999999995</v>
-      </c>
-    </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E35" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F35" s="4">
-        <v>2.69</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="0"/>
-        <v>6.8326000000000002</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L59"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
@@ -4751,10 +4324,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="43"/>
+      <c r="C1" s="41"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
@@ -4815,17 +4388,17 @@
       <c r="C7" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="48" t="s">
         <v>356</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
     </row>
     <row r="8" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
@@ -4834,15 +4407,15 @@
       <c r="C8" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
     </row>
     <row r="9" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
@@ -4851,15 +4424,15 @@
       <c r="C9" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
@@ -4880,12 +4453,12 @@
       <c r="C11" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="40" t="s">
         <v>229</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4895,10 +4468,10 @@
       <c r="C12" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
@@ -4968,10 +4541,10 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="42" t="s">
         <v>364</v>
       </c>
-      <c r="C19" s="44"/>
+      <c r="C19" s="42"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -5025,10 +4598,10 @@
       <c r="B24" s="23"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="39" t="s">
         <v>365</v>
       </c>
-      <c r="C25" s="45"/>
+      <c r="C25" s="39"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="23" t="s">
@@ -5066,50 +4639,50 @@
       <c r="B30" s="23"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="39" t="s">
         <v>366</v>
       </c>
-      <c r="C31" s="45"/>
+      <c r="C31" s="39"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="40" t="s">
         <v>367</v>
       </c>
-      <c r="C32" s="28"/>
+      <c r="C32" s="40"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
     </row>
     <row r="34" spans="2:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="35" t="s">
         <v>308</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="36" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="128" x14ac:dyDescent="0.2">
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="35" t="s">
         <v>275</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="37" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="35" t="s">
         <v>276</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="31" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="112" x14ac:dyDescent="0.2">
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="38" t="s">
         <v>371</v>
       </c>
     </row>
@@ -5117,14 +4690,14 @@
       <c r="B38" s="23"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
@@ -5133,13 +4706,13 @@
       <c r="C41" t="s">
         <v>230</v>
       </c>
-      <c r="D41" s="27" t="s">
+      <c r="D41" s="45" t="s">
         <v>307</v>
       </c>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
@@ -5148,13 +4721,13 @@
       <c r="C42" t="s">
         <v>231</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="D42" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
@@ -5165,13 +4738,13 @@
       <c r="C43" t="s">
         <v>232</v>
       </c>
-      <c r="D43" s="27" t="s">
+      <c r="D43" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
@@ -5180,19 +4753,19 @@
       <c r="C44" t="s">
         <v>233</v>
       </c>
-      <c r="D44" s="27" t="s">
+      <c r="D44" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="47"/>
+      <c r="C46" s="46"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
@@ -5251,10 +4824,10 @@
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="48" t="s">
+      <c r="B55" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="48"/>
+      <c r="C55" s="43"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -5264,36 +4837,36 @@
       <c r="B56" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="26" t="s">
+      <c r="C56" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="26" t="s">
+      <c r="C57" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="26"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.2">
@@ -5310,11 +4883,9 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C33"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="D11:G12"/>
+    <mergeCell ref="D7:L9"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="C58:F58"/>
     <mergeCell ref="C57:G57"/>
@@ -5324,9 +4895,11 @@
     <mergeCell ref="D43:H43"/>
     <mergeCell ref="D44:H44"/>
     <mergeCell ref="D42:H42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="D11:G12"/>
-    <mergeCell ref="D7:L9"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C33"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed code to convert data into matrix form. Completed code to generate heatmaps. Last Step in progress: Currently working on how to structure the code to allow easy combination of data by functional type.
</commit_message>
<xml_diff>
--- a/Data/VegData.xlsx
+++ b/Data/VegData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lina/Documents/GitHub/Model/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elise\Desktop\GitHub\sparrow925.github.io\Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="440" yWindow="580" windowWidth="26880" windowHeight="13600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="435" yWindow="585" windowWidth="26880" windowHeight="13605" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="372">
   <si>
     <t>SN</t>
   </si>
@@ -1208,8 +1208,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1457,17 +1457,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1481,11 +1478,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1770,33 +1770,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="101" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="14" width="10.5" style="4" customWidth="1"/>
-    <col min="15" max="15" width="9.83203125" style="4" customWidth="1"/>
+    <col min="6" max="14" width="10.44140625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="9.77734375" style="4" customWidth="1"/>
     <col min="16" max="16" width="11.33203125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="10.5" style="4" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" style="4" customWidth="1"/>
     <col min="18" max="18" width="9.6640625" style="4" customWidth="1"/>
     <col min="19" max="19" width="31.33203125" style="28" customWidth="1"/>
     <col min="20" max="20" width="39" style="25" customWidth="1"/>
-    <col min="21" max="21" width="23.5" style="22" customWidth="1"/>
-    <col min="22" max="22" width="24.1640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" style="22" customWidth="1"/>
+    <col min="22" max="22" width="24.109375" style="2" customWidth="1"/>
     <col min="23" max="23" width="28.33203125" style="23" customWidth="1"/>
     <col min="24" max="24" width="35" style="1" customWidth="1"/>
     <col min="25" max="25" width="30.33203125" style="23" customWidth="1"/>
     <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="10" customFormat="1" ht="31.5">
       <c r="A1" s="7" t="s">
         <v>109</v>
       </c>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="Z1" s="7"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26">
       <c r="A2" s="4" t="s">
         <v>172</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26">
       <c r="A3" s="4">
         <v>20</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26">
       <c r="A4" s="4">
         <v>19</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26">
       <c r="A5" s="4" t="s">
         <v>172</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26">
       <c r="A6" s="4" t="s">
         <v>172</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26">
       <c r="A7" s="4" t="s">
         <v>172</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26">
       <c r="A8" s="4">
         <v>19</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26">
       <c r="A9" s="4">
         <v>19</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26">
       <c r="A10" s="4" t="s">
         <v>172</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26">
       <c r="A11" s="4">
         <v>19</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26">
       <c r="A12" s="4">
         <v>20</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26">
       <c r="A13" s="4">
         <v>20</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26">
       <c r="A14" s="4">
         <v>19</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26">
       <c r="A15" s="4">
         <v>19</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26">
       <c r="A16" s="4">
         <v>19</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25">
       <c r="A17" s="4" t="s">
         <v>172</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25">
       <c r="A18" s="4">
         <v>19</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25">
       <c r="A19" s="4">
         <v>20</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25">
       <c r="A20" s="4" t="s">
         <v>172</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25">
       <c r="A21" s="4" t="s">
         <v>172</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25">
       <c r="A22" s="4">
         <v>19</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25">
       <c r="A23" s="4">
         <v>19</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25">
       <c r="A24" s="4" t="s">
         <v>172</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25">
       <c r="A25" s="4">
         <v>19</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25">
       <c r="A26" s="4">
         <v>19</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25">
       <c r="A27" s="4" t="s">
         <v>172</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25">
       <c r="A28" s="4">
         <v>19</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25">
       <c r="A29" s="4">
         <v>20</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25">
       <c r="A30" s="4">
         <v>20</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25">
       <c r="A31" s="4">
         <v>20</v>
       </c>
@@ -3942,9 +3942,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
-        <v>19</v>
+    <row r="32" spans="1:25">
+      <c r="A32" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>165</v>
@@ -4013,7 +4013,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25">
       <c r="A33" s="4" t="s">
         <v>172</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25">
       <c r="A34" s="4" t="s">
         <v>172</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25">
       <c r="A35" s="4">
         <v>20</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="5"/>
@@ -4226,7 +4226,7 @@
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="5"/>
@@ -4241,7 +4241,7 @@
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="5"/>
@@ -4256,7 +4256,7 @@
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="5"/>
@@ -4271,7 +4271,7 @@
       <c r="L40" s="12"/>
       <c r="M40" s="12"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="5"/>
@@ -4311,26 +4311,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
     <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="2:12" ht="15.75">
+      <c r="B1" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="41"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12">
       <c r="B2" s="16" t="s">
         <v>109</v>
       </c>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:12">
       <c r="B3" s="16" t="s">
         <v>166</v>
       </c>
@@ -4348,7 +4348,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -4381,60 +4381,60 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" ht="18.95" customHeight="1">
       <c r="B7" s="10" t="s">
         <v>352</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="41" t="s">
         <v>356</v>
       </c>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-    </row>
-    <row r="8" spans="2:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+    </row>
+    <row r="8" spans="2:12" ht="23.1" customHeight="1">
       <c r="B8" s="10" t="s">
         <v>353</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-    </row>
-    <row r="9" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+    </row>
+    <row r="9" spans="2:12" ht="26.1" customHeight="1">
       <c r="B9" s="10" t="s">
         <v>261</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10" s="10" t="s">
         <v>262</v>
       </c>
@@ -4446,7 +4446,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" ht="27" customHeight="1">
       <c r="B11" s="10" t="s">
         <v>348</v>
       </c>
@@ -4461,7 +4461,7 @@
       <c r="G11" s="40"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" ht="24" customHeight="1">
       <c r="B12" s="10" t="s">
         <v>349</v>
       </c>
@@ -4474,7 +4474,7 @@
       <c r="G12" s="40"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12">
       <c r="B13" t="s">
         <v>188</v>
       </c>
@@ -4486,7 +4486,7 @@
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12">
       <c r="B14" t="s">
         <v>168</v>
       </c>
@@ -4498,7 +4498,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12">
       <c r="B15" t="s">
         <v>171</v>
       </c>
@@ -4510,7 +4510,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B16" t="s">
         <v>169</v>
       </c>
@@ -4522,7 +4522,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8">
       <c r="B17" t="s">
         <v>170</v>
       </c>
@@ -4534,23 +4534,23 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="42" t="s">
+    <row r="19" spans="2:8" ht="15.75">
+      <c r="B19" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="C19" s="42"/>
+      <c r="C19" s="48"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B20" s="2">
         <v>1</v>
       </c>
@@ -4562,7 +4562,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="2">
         <v>2</v>
       </c>
@@ -4574,7 +4574,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8">
       <c r="B22" s="2">
         <v>3</v>
       </c>
@@ -4586,7 +4586,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8">
       <c r="B23" s="2" t="s">
         <v>148</v>
       </c>
@@ -4594,16 +4594,16 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8">
       <c r="B24" s="23"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="39" t="s">
+    <row r="25" spans="2:8" ht="15.75">
+      <c r="B25" s="46" t="s">
         <v>365</v>
       </c>
-      <c r="C25" s="39"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C25" s="46"/>
+    </row>
+    <row r="26" spans="2:8">
       <c r="B26" s="23" t="s">
         <v>271</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8">
       <c r="B27" s="23" t="s">
         <v>299</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8">
       <c r="B28" s="23" t="s">
         <v>272</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8">
       <c r="B29" s="23" t="s">
         <v>281</v>
       </c>
@@ -4635,26 +4635,26 @@
         <v>363</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8">
       <c r="B30" s="23"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="39" t="s">
+    <row r="31" spans="2:8" ht="15.75">
+      <c r="B31" s="46" t="s">
         <v>366</v>
       </c>
-      <c r="C31" s="39"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C31" s="46"/>
+    </row>
+    <row r="32" spans="2:8">
       <c r="B32" s="40" t="s">
         <v>367</v>
       </c>
       <c r="C32" s="40"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10">
       <c r="B33" s="40"/>
       <c r="C33" s="40"/>
     </row>
-    <row r="34" spans="2:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" ht="75.75">
       <c r="B34" s="35" t="s">
         <v>308</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="128" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" ht="110.25">
       <c r="B35" s="35" t="s">
         <v>275</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" ht="90.75">
       <c r="B36" s="35" t="s">
         <v>276</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" ht="78.75">
       <c r="B37" s="35" t="s">
         <v>290</v>
       </c>
@@ -4686,88 +4686,88 @@
         <v>371</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10">
       <c r="B38" s="23"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B40" s="47" t="s">
+    <row r="40" spans="2:10" ht="15.75">
+      <c r="B40" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+    </row>
+    <row r="41" spans="2:10">
       <c r="B41" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C41" t="s">
         <v>230</v>
       </c>
-      <c r="D41" s="45" t="s">
+      <c r="D41" s="44" t="s">
         <v>307</v>
       </c>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+    </row>
+    <row r="42" spans="2:10">
       <c r="B42" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C42" t="s">
         <v>231</v>
       </c>
-      <c r="D42" s="45" t="s">
+      <c r="D42" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10">
       <c r="B43" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C43" t="s">
         <v>232</v>
       </c>
-      <c r="D43" s="45" t="s">
+      <c r="D43" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+    </row>
+    <row r="44" spans="2:10">
       <c r="B44" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C44" t="s">
         <v>233</v>
       </c>
-      <c r="D44" s="45" t="s">
+      <c r="D44" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="46" t="s">
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+    </row>
+    <row r="46" spans="2:10" ht="15.75">
+      <c r="B46" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="46"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C46" s="45"/>
+    </row>
+    <row r="47" spans="2:10">
       <c r="B47" t="s">
         <v>57</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10">
       <c r="B48" t="s">
         <v>56</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:7">
       <c r="B49" t="s">
         <v>59</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7">
       <c r="B50" t="s">
         <v>66</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:7">
       <c r="B51" t="s">
         <v>58</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:7">
       <c r="B52" t="s">
         <v>61</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:7">
       <c r="B53" t="s">
         <v>62</v>
       </c>
@@ -4823,53 +4823,53 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="43" t="s">
+    <row r="55" spans="2:7" ht="15.75">
+      <c r="B55" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="43"/>
+      <c r="C55" s="42"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:7">
       <c r="B56" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="44" t="s">
+      <c r="C56" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="D56" s="44"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="44"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+    </row>
+    <row r="57" spans="2:7">
       <c r="B57" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="44" t="s">
+      <c r="C57" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="44"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+    </row>
+    <row r="58" spans="2:7">
       <c r="B58" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C58" s="44" t="s">
+      <c r="C58" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="D58" s="44"/>
-      <c r="E58" s="44"/>
-      <c r="F58" s="44"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:7">
       <c r="B59" s="3" t="s">
         <v>148</v>
       </c>
@@ -4883,6 +4883,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B40:G40"/>
     <mergeCell ref="D11:G12"/>
     <mergeCell ref="D7:L9"/>
@@ -4898,8 +4900,6 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C33"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>